<commit_message>
Final results 5.1 pcpp
</commit_message>
<xml_diff>
--- a/Source/8 Practical Concurrent and Parallel Programming/Week5/results/jve_5.1.1-5.1.2.xlsx
+++ b/Source/8 Practical Concurrent and Parallel Programming/Week5/results/jve_5.1.1-5.1.2.xlsx
@@ -1,32 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITU programming\Shared\Source\8 Practical Concurrent and Parallel Programming\Week5\results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17408" windowHeight="9810"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
-    <t># of tasks</t>
+    <t>CachedThreadPool</t>
+  </si>
+  <si>
+    <t>WorkStealingPool</t>
   </si>
   <si>
     <t>Shared</t>
@@ -35,10 +31,7 @@
     <t>Local</t>
   </si>
   <si>
-    <t>WorkStealingPool</t>
-  </si>
-  <si>
-    <t>CachedThreadPool</t>
+    <t># of tasks</t>
   </si>
 </sst>
 </file>
@@ -76,16 +69,16 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -519,304 +512,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>11480.5</c:v>
+                  <c:v>9340.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7222.2</c:v>
+                  <c:v>5787.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5282.5</c:v>
+                  <c:v>4150.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4318.3999999999996</c:v>
+                  <c:v>3195.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4524</c:v>
+                  <c:v>4322.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4099.8</c:v>
+                  <c:v>3878</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3435.8</c:v>
+                  <c:v>3214.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2961.7</c:v>
+                  <c:v>2749.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3570.9</c:v>
+                  <c:v>3322</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3457.8</c:v>
+                  <c:v>3116.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3195.4</c:v>
+                  <c:v>2869.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3053</c:v>
+                  <c:v>2710.7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3405.3</c:v>
+                  <c:v>3278.9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3189.5</c:v>
+                  <c:v>3057.7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2971.1</c:v>
+                  <c:v>2809.4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2785.4</c:v>
+                  <c:v>2614</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3105.3</c:v>
+                  <c:v>2932.9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3032.4</c:v>
+                  <c:v>2829.8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2921.2</c:v>
+                  <c:v>2710.3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2862.9</c:v>
+                  <c:v>2629.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3057</c:v>
+                  <c:v>2944.6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2949.3</c:v>
+                  <c:v>2828.2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2825.9</c:v>
+                  <c:v>2682.3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2720.6</c:v>
+                  <c:v>2572.9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2930</c:v>
+                  <c:v>2786.6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2867.4</c:v>
+                  <c:v>2710.3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2797.1</c:v>
+                  <c:v>2619.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2775.2</c:v>
+                  <c:v>2574.9</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2917.7</c:v>
+                  <c:v>2773.2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2846.3</c:v>
+                  <c:v>2738.1</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2758.9</c:v>
+                  <c:v>2631.7</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2686.3</c:v>
+                  <c:v>2547.9</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2845.1</c:v>
+                  <c:v>2718.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2786.3</c:v>
+                  <c:v>2650.4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2744.6</c:v>
+                  <c:v>2585</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2730.5</c:v>
+                  <c:v>2553.1</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2836.4</c:v>
+                  <c:v>2726</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2794.1</c:v>
+                  <c:v>2665.4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2724.3</c:v>
+                  <c:v>2589.9</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2672.4</c:v>
+                  <c:v>2535.1</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2789.7</c:v>
+                  <c:v>2684.8</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2773.9</c:v>
+                  <c:v>2664.5</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2725.7</c:v>
+                  <c:v>2570.1</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2705.6</c:v>
+                  <c:v>2547.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2783.7</c:v>
+                  <c:v>2667.8</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2752.5</c:v>
+                  <c:v>2630</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2694.4</c:v>
+                  <c:v>2586.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2658.6</c:v>
+                  <c:v>2532.4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2767.5</c:v>
+                  <c:v>2643.9</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2759.4</c:v>
+                  <c:v>2593.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2690.9</c:v>
+                  <c:v>2554.4</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2676.3</c:v>
+                  <c:v>2534.9</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2740</c:v>
+                  <c:v>2629.1</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2713</c:v>
+                  <c:v>2609.1</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2673.6</c:v>
+                  <c:v>2555.5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2662.7</c:v>
+                  <c:v>2530.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2743.6</c:v>
+                  <c:v>2614.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2694.3</c:v>
+                  <c:v>2572.9</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2688.7</c:v>
+                  <c:v>2556.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2706.9</c:v>
+                  <c:v>2536.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2718</c:v>
+                  <c:v>2611.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2716.2</c:v>
+                  <c:v>2586.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2674.7</c:v>
+                  <c:v>2548.6</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2649.9</c:v>
+                  <c:v>2526.4</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2701.9</c:v>
+                  <c:v>2598.4</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>2698.9</c:v>
+                  <c:v>2572.1</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>2669.7</c:v>
+                  <c:v>2544.6</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>2679</c:v>
+                  <c:v>2531.1</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2689</c:v>
+                  <c:v>2583.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2680.7</c:v>
+                  <c:v>2560.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2657.8</c:v>
+                  <c:v>2539.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>2653.8</c:v>
+                  <c:v>2532.5</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>2681.3</c:v>
+                  <c:v>2566.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>2664</c:v>
+                  <c:v>2547.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>2710.5</c:v>
+                  <c:v>2537.9</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>2675.8</c:v>
+                  <c:v>2534.6</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>2678.3</c:v>
+                  <c:v>2566.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>2663.1</c:v>
+                  <c:v>2563.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>2658.2</c:v>
+                  <c:v>2539.5</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>2639.6</c:v>
+                  <c:v>2517.4</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>2685.3</c:v>
+                  <c:v>2572.6</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2669.1</c:v>
+                  <c:v>2549.6</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2675.2</c:v>
+                  <c:v>2534.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>2689</c:v>
+                  <c:v>2549.5</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>2673.4</c:v>
+                  <c:v>2564.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>2678</c:v>
+                  <c:v>2552.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>2650.1</c:v>
+                  <c:v>2545.4</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2652</c:v>
+                  <c:v>2535.4</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2670.4</c:v>
+                  <c:v>2560.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>2647.4</c:v>
+                  <c:v>2531.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2642</c:v>
+                  <c:v>2523.6</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2669.1</c:v>
+                  <c:v>2549.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>2665.3</c:v>
+                  <c:v>2545</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2675.2</c:v>
+                  <c:v>2549.5</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>2647</c:v>
+                  <c:v>2535.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>2642.6</c:v>
+                  <c:v>2524.6</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2674.8</c:v>
+                  <c:v>2600.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2644.8</c:v>
+                  <c:v>2535.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2655.2</c:v>
+                  <c:v>2527.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2664.4</c:v>
+                  <c:v>2527.3000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1169,304 +1162,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>11499.6</c:v>
+                  <c:v>9461.2000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7205.5</c:v>
+                  <c:v>5954.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5302.6</c:v>
+                  <c:v>5201.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4682.5</c:v>
+                  <c:v>4725.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4574</c:v>
+                  <c:v>4710.3999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4089.1</c:v>
+                  <c:v>4183.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3472.3</c:v>
+                  <c:v>3539.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2980.2</c:v>
+                  <c:v>3076.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3602.4</c:v>
+                  <c:v>3709.7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3463.2</c:v>
+                  <c:v>3563.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3223</c:v>
+                  <c:v>3347.9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3068</c:v>
+                  <c:v>3201.6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3398.6</c:v>
+                  <c:v>3473.7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3220.3</c:v>
+                  <c:v>3302.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2990.1</c:v>
+                  <c:v>3114.8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2801</c:v>
+                  <c:v>2953</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3127.4</c:v>
+                  <c:v>3216.1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3052.8</c:v>
+                  <c:v>3203.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2951.7</c:v>
+                  <c:v>3198.6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2869.3</c:v>
+                  <c:v>3196.7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3100.3</c:v>
+                  <c:v>3196.4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2979.3</c:v>
+                  <c:v>3158.2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2845.4</c:v>
+                  <c:v>3090.3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2741.6</c:v>
+                  <c:v>3035.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2953</c:v>
+                  <c:v>3204.8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2896</c:v>
+                  <c:v>3204.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2823.2</c:v>
+                  <c:v>3215.8</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2789.8</c:v>
+                  <c:v>3225.2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2942.3</c:v>
+                  <c:v>3196.7</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2865.1</c:v>
+                  <c:v>3151.9</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2807.9</c:v>
+                  <c:v>3096.4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2707.6</c:v>
+                  <c:v>3066.4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2873.9</c:v>
+                  <c:v>3167.5</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2815.4</c:v>
+                  <c:v>3168.7</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2773.2</c:v>
+                  <c:v>3162.8</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2752.2</c:v>
+                  <c:v>3160.6</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2852</c:v>
+                  <c:v>3140.7</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2810.2</c:v>
+                  <c:v>3110.5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2743.1</c:v>
+                  <c:v>3066.8</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2693.8</c:v>
+                  <c:v>3054.5</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2812.5</c:v>
+                  <c:v>3106.1</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2784.1</c:v>
+                  <c:v>3123.1</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2741.2</c:v>
+                  <c:v>3120.1</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2733.6</c:v>
+                  <c:v>3104.6</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2797</c:v>
+                  <c:v>3084.8</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2770.3</c:v>
+                  <c:v>3057.7</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2720.3</c:v>
+                  <c:v>3025.8</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2685.7</c:v>
+                  <c:v>3011.4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2785</c:v>
+                  <c:v>3072.1</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2737.5</c:v>
+                  <c:v>3066.1</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2714.4</c:v>
+                  <c:v>3054.8</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2727.6</c:v>
+                  <c:v>3054.1</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2748.4</c:v>
+                  <c:v>3039</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2728.9</c:v>
+                  <c:v>3010.3</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2702.5</c:v>
+                  <c:v>3002</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2691</c:v>
+                  <c:v>3012.5</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2755.4</c:v>
+                  <c:v>3040.5</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2713.1</c:v>
+                  <c:v>3030.8</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2709.5</c:v>
+                  <c:v>3064.1</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2732.5</c:v>
+                  <c:v>3043.6</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2722.3</c:v>
+                  <c:v>3010.1</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2712.1</c:v>
+                  <c:v>2996.1</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2690.8</c:v>
+                  <c:v>2991.3</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2674.6</c:v>
+                  <c:v>2968.6</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2722.4</c:v>
+                  <c:v>2999.5</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>2707.3</c:v>
+                  <c:v>3004.8</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>2688.9</c:v>
+                  <c:v>3007.1</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>2722.5</c:v>
+                  <c:v>2988.1</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2693.5</c:v>
+                  <c:v>2983.5</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2701</c:v>
+                  <c:v>2973.8</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2678.6</c:v>
+                  <c:v>2957.7</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>2671.5</c:v>
+                  <c:v>2959.6</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>2699.5</c:v>
+                  <c:v>2978</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>2684.7</c:v>
+                  <c:v>2978.9</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>2671.7</c:v>
+                  <c:v>2982.2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>2706.1</c:v>
+                  <c:v>2978.4</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>2694.5</c:v>
+                  <c:v>2973.7</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>2685.8</c:v>
+                  <c:v>2962.6</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>2677.3</c:v>
+                  <c:v>2961</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>2658.8</c:v>
+                  <c:v>2944</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>2706.3</c:v>
+                  <c:v>2978.1</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2698.1</c:v>
+                  <c:v>2978.6</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2739.4</c:v>
+                  <c:v>2985.2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>2707.1</c:v>
+                  <c:v>2987.8</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>2697.9</c:v>
+                  <c:v>2971.1</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>2700.7</c:v>
+                  <c:v>2972.2</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>2670.1</c:v>
+                  <c:v>2958.7</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2660</c:v>
+                  <c:v>2953.5</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2696.3</c:v>
+                  <c:v>2969.3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>2690.4</c:v>
+                  <c:v>2961.9</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2660.5</c:v>
+                  <c:v>2966.7</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2695.9</c:v>
+                  <c:v>2960.3</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>2675.9</c:v>
+                  <c:v>2957.2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2690.1</c:v>
+                  <c:v>2968.8</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>2670.3</c:v>
+                  <c:v>2958</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>2660.4</c:v>
+                  <c:v>2954.5</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2693.2</c:v>
+                  <c:v>2972.7</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2672</c:v>
+                  <c:v>2964.8</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2669.7</c:v>
+                  <c:v>2956.6</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2675.7</c:v>
+                  <c:v>2960.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1819,304 +1812,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>11418.7</c:v>
+                  <c:v>9261</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7185.2</c:v>
+                  <c:v>5780.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5255.9</c:v>
+                  <c:v>4871.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4046.8</c:v>
+                  <c:v>4063.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4661.6000000000004</c:v>
+                  <c:v>4602.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3979.1</c:v>
+                  <c:v>3943.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3323.1</c:v>
+                  <c:v>3335.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3092.1</c:v>
+                  <c:v>3103.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3470.1</c:v>
+                  <c:v>3418.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3353.8</c:v>
+                  <c:v>3226.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3165.8</c:v>
+                  <c:v>2999.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3275.5</c:v>
+                  <c:v>2895.3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3244</c:v>
+                  <c:v>3073.4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3179.4</c:v>
+                  <c:v>2925.6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3090.3</c:v>
+                  <c:v>2760.1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2906.7</c:v>
+                  <c:v>2689.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3001.2</c:v>
+                  <c:v>2814.1</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2984.3</c:v>
+                  <c:v>2751.8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2904.1</c:v>
+                  <c:v>2690.3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2885.1</c:v>
+                  <c:v>2701.9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2954.5</c:v>
+                  <c:v>2798.3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2891.6</c:v>
+                  <c:v>2722.8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2781.5</c:v>
+                  <c:v>2643.6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2775.3</c:v>
+                  <c:v>2624</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2845</c:v>
+                  <c:v>2691.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2838.2</c:v>
+                  <c:v>2659.8</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2790.5</c:v>
+                  <c:v>2619</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2798</c:v>
+                  <c:v>2642.3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2834.9</c:v>
+                  <c:v>2689.1</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2793.2</c:v>
+                  <c:v>2647.8</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2729.1</c:v>
+                  <c:v>2600.1</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2733.3</c:v>
+                  <c:v>2594.4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2770.6</c:v>
+                  <c:v>2637.4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2774.7</c:v>
+                  <c:v>2614.1</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2766</c:v>
+                  <c:v>2587.9</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2785.6</c:v>
+                  <c:v>2641.8</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2775.3</c:v>
+                  <c:v>2651.2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2750.8</c:v>
+                  <c:v>2613.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2707.1</c:v>
+                  <c:v>2578.9</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2737</c:v>
+                  <c:v>2580.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2742.4</c:v>
+                  <c:v>2611.6</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2732.6</c:v>
+                  <c:v>2600.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2715.3</c:v>
+                  <c:v>2587.4</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2734.5</c:v>
+                  <c:v>2634.3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2745.4</c:v>
+                  <c:v>2623.8</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2724</c:v>
+                  <c:v>2607.1</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2689</c:v>
+                  <c:v>2583.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2702.8</c:v>
+                  <c:v>2584.4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2718</c:v>
+                  <c:v>2612.5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2704.1</c:v>
+                  <c:v>2585.4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2687.5</c:v>
+                  <c:v>2581</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2702</c:v>
+                  <c:v>2599.1</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2717.8</c:v>
+                  <c:v>2610.6</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2686.9</c:v>
+                  <c:v>2598.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2676.3</c:v>
+                  <c:v>2577.6</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2703.4</c:v>
+                  <c:v>2592.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2707</c:v>
+                  <c:v>3423.9</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2692.2</c:v>
+                  <c:v>2708.3</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2695.1</c:v>
+                  <c:v>2686</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2696</c:v>
+                  <c:v>2626.9</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2701</c:v>
+                  <c:v>2610.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2677.5</c:v>
+                  <c:v>2603.5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2665.3</c:v>
+                  <c:v>2585.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2689.7</c:v>
+                  <c:v>2597.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2686.4</c:v>
+                  <c:v>2607.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>2680.1</c:v>
+                  <c:v>2603.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>2672.4</c:v>
+                  <c:v>2604.1</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>2691.7</c:v>
+                  <c:v>2615.1</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2685.6</c:v>
+                  <c:v>2612.5</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2676.5</c:v>
+                  <c:v>2606.6</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2671.7</c:v>
+                  <c:v>2594.1</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>2702.6</c:v>
+                  <c:v>2608.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>2686.2</c:v>
+                  <c:v>2614.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>2674.9</c:v>
+                  <c:v>2606.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>2669.7</c:v>
+                  <c:v>2602.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>2682.5</c:v>
+                  <c:v>2618.4</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>2679.1</c:v>
+                  <c:v>2619.4</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>2669.8</c:v>
+                  <c:v>2604.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>2668.2</c:v>
+                  <c:v>2599.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>2679.4</c:v>
+                  <c:v>2646.7</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>2672</c:v>
+                  <c:v>2650.8</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2680.4</c:v>
+                  <c:v>2644.5</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2671.9</c:v>
+                  <c:v>2606.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>2654.3</c:v>
+                  <c:v>2599.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>2670.8</c:v>
+                  <c:v>2616.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>2673.6</c:v>
+                  <c:v>2616.4</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>2662.9</c:v>
+                  <c:v>2609.1</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2660.7</c:v>
+                  <c:v>2602.6</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2681.8</c:v>
+                  <c:v>2613.9</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>2675.5</c:v>
+                  <c:v>2616.1</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2665.3</c:v>
+                  <c:v>2612.5</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2662.7</c:v>
+                  <c:v>2609.5</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>2658.8</c:v>
+                  <c:v>2614.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2695.4</c:v>
+                  <c:v>2623.6</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>2668.1</c:v>
+                  <c:v>2615.9</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>2669</c:v>
+                  <c:v>2611.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2669.7</c:v>
+                  <c:v>2612.9</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2667.3</c:v>
+                  <c:v>2623.1</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2685.6</c:v>
+                  <c:v>2619.9</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2661.1</c:v>
+                  <c:v>2612</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2475,304 +2468,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>11561.6</c:v>
+                  <c:v>9365.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7255.1</c:v>
+                  <c:v>5971.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5249.6</c:v>
+                  <c:v>4337.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4154.2</c:v>
+                  <c:v>3392.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4740.7</c:v>
+                  <c:v>4375.1000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4019.4</c:v>
+                  <c:v>3721.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3373.1</c:v>
+                  <c:v>3179.8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3141.9</c:v>
+                  <c:v>2993.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3509.8</c:v>
+                  <c:v>3061.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3420.7</c:v>
+                  <c:v>3109.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3347</c:v>
+                  <c:v>3197.7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3104</c:v>
+                  <c:v>3151.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3316.1</c:v>
+                  <c:v>3152.3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3116.3</c:v>
+                  <c:v>3110.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2907.6</c:v>
+                  <c:v>3029</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2834.5</c:v>
+                  <c:v>3008.1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2900.5</c:v>
+                  <c:v>2994.4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2859.9</c:v>
+                  <c:v>2988.1</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2796.3</c:v>
+                  <c:v>2990.2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2782.9</c:v>
+                  <c:v>2996.7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2729.9</c:v>
+                  <c:v>2984.4</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2676.4</c:v>
+                  <c:v>2963.3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2612.9</c:v>
+                  <c:v>2941.6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2612.9</c:v>
+                  <c:v>2918.8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2603.5</c:v>
+                  <c:v>2907.3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2591.1999999999998</c:v>
+                  <c:v>2899.2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2589.1999999999998</c:v>
+                  <c:v>2898</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2604.4</c:v>
+                  <c:v>2898.4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2591.5</c:v>
+                  <c:v>2899.3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2593.6999999999998</c:v>
+                  <c:v>2884.6</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2567.5</c:v>
+                  <c:v>2880.6</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2567.1</c:v>
+                  <c:v>2868.2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2682.9</c:v>
+                  <c:v>2867.6</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2588.6</c:v>
+                  <c:v>2861.1</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2590.6999999999998</c:v>
+                  <c:v>2854.4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2577.6</c:v>
+                  <c:v>2860.7</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2554</c:v>
+                  <c:v>2854.7</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2531.9</c:v>
+                  <c:v>2851.9</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2511.6999999999998</c:v>
+                  <c:v>2877.5</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2506.9</c:v>
+                  <c:v>2842.9</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2495.9</c:v>
+                  <c:v>2838.9</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2493.6</c:v>
+                  <c:v>2831.4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2492.9</c:v>
+                  <c:v>2830.1</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2478.9</c:v>
+                  <c:v>2831.7</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2465.1</c:v>
+                  <c:v>2831.9</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2456.1999999999998</c:v>
+                  <c:v>2830</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2436</c:v>
+                  <c:v>2841.2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2440</c:v>
+                  <c:v>2830.3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2437.8000000000002</c:v>
+                  <c:v>2831.6</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2426.4</c:v>
+                  <c:v>2824.3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2427.6</c:v>
+                  <c:v>2824.4</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2442.4</c:v>
+                  <c:v>2824.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2421.5</c:v>
+                  <c:v>2822.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2410.8000000000002</c:v>
+                  <c:v>2822.3</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2416.1</c:v>
+                  <c:v>2823.5</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2430.1</c:v>
+                  <c:v>2825</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2419.6999999999998</c:v>
+                  <c:v>2824</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2419</c:v>
+                  <c:v>2826.4</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2407.3000000000002</c:v>
+                  <c:v>2827.8</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2406.4</c:v>
+                  <c:v>2823.8</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2373.5</c:v>
+                  <c:v>2850.7</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2374.6999999999998</c:v>
+                  <c:v>2827.2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2361</c:v>
+                  <c:v>2827.2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2355.3000000000002</c:v>
+                  <c:v>2824.2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2351.9</c:v>
+                  <c:v>2824.5</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>2343.8000000000002</c:v>
+                  <c:v>2828</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>2342.6</c:v>
+                  <c:v>2828.4</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>2345.5</c:v>
+                  <c:v>2828.5</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2337.1</c:v>
+                  <c:v>2826.6</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2335</c:v>
+                  <c:v>2829.8</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2325.1</c:v>
+                  <c:v>2829.4</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>2333.9</c:v>
+                  <c:v>2831.5</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>2326.9</c:v>
+                  <c:v>3010.2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>2322.1999999999998</c:v>
+                  <c:v>3070.8</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>2310.4</c:v>
+                  <c:v>3073.8</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>2319.8000000000002</c:v>
+                  <c:v>3088.3</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>2312.6</c:v>
+                  <c:v>2867.3</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>2305.1999999999998</c:v>
+                  <c:v>2833.1</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>2299.6</c:v>
+                  <c:v>2833.1</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>2292.4</c:v>
+                  <c:v>2836</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>2290.4</c:v>
+                  <c:v>2837.9</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>2300.9</c:v>
+                  <c:v>2841.1</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>2302.5</c:v>
+                  <c:v>2838.7</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>2287.6999999999998</c:v>
+                  <c:v>2839</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>2282.9</c:v>
+                  <c:v>2841.5</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>2281.9</c:v>
+                  <c:v>2838.2</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>2278.4</c:v>
+                  <c:v>2836.7</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2280.6999999999998</c:v>
+                  <c:v>2838.6</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2283.1</c:v>
+                  <c:v>2843.2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>2291.8000000000002</c:v>
+                  <c:v>2841.6</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2311.3000000000002</c:v>
+                  <c:v>2839.4</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2285.1999999999998</c:v>
+                  <c:v>2894.6</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>2290.9</c:v>
+                  <c:v>2857.4</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2293.4</c:v>
+                  <c:v>2880</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>2301.1999999999998</c:v>
+                  <c:v>2842.9</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>2281.1</c:v>
+                  <c:v>2842.1</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2278.4</c:v>
+                  <c:v>2845.8</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2269.5</c:v>
+                  <c:v>2844</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2264.3000000000002</c:v>
+                  <c:v>2844.1</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2262.1</c:v>
+                  <c:v>2844.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2789,11 +2782,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-764739056"/>
-        <c:axId val="-764739600"/>
+        <c:axId val="2014856304"/>
+        <c:axId val="2014858480"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-764739056"/>
+        <c:axId val="2014856304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2906,7 +2899,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-764739600"/>
+        <c:crossAx val="2014858480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2914,7 +2907,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-764739600"/>
+        <c:axId val="2014858480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3021,7 +3014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-764739056"/>
+        <c:crossAx val="2014856304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3650,20 +3643,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9523</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>19047</xdr:rowOff>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>114302</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>176213</xdr:rowOff>
+      <xdr:rowOff>52391</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagram 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3680,6 +3675,520 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Ark1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="A3">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>12</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>13</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>14</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>15</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>16</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>17</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>18</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>19</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>20</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>21</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>22</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>23</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>24</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>25</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>26</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>27</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>28</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>29</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>30</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>31</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>32</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>33</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>34</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>36</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>37</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>38</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>39</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>40</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>41</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>42</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>43</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>44</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>45</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>46</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>47</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>48</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>49</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52">
+            <v>50</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53">
+            <v>51</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54">
+            <v>52</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55">
+            <v>53</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56">
+            <v>54</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57">
+            <v>55</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58">
+            <v>56</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59">
+            <v>57</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60">
+            <v>58</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61">
+            <v>59</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62">
+            <v>60</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63">
+            <v>61</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64">
+            <v>62</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65">
+            <v>63</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66">
+            <v>64</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67">
+            <v>65</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68">
+            <v>66</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69">
+            <v>67</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70">
+            <v>68</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71">
+            <v>69</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72">
+            <v>70</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73">
+            <v>71</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74">
+            <v>72</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75">
+            <v>73</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76">
+            <v>74</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77">
+            <v>75</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78">
+            <v>76</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79">
+            <v>77</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80">
+            <v>78</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81">
+            <v>79</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82">
+            <v>80</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83">
+            <v>81</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84">
+            <v>82</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85">
+            <v>83</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86">
+            <v>84</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87">
+            <v>85</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88">
+            <v>86</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89">
+            <v>87</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90">
+            <v>88</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91">
+            <v>89</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92">
+            <v>90</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93">
+            <v>91</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94">
+            <v>92</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95">
+            <v>93</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96">
+            <v>94</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97">
+            <v>95</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98">
+            <v>96</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99">
+            <v>97</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100">
+            <v>98</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101">
+            <v>99</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102">
+            <v>100</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
@@ -3691,39 +4200,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Kontor">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3802,422 +4311,442 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>11561.6</v>
+        <v>9365.5</v>
       </c>
       <c r="C3">
-        <v>11418.7</v>
+        <v>9261</v>
       </c>
       <c r="D3">
-        <v>11499.6</v>
+        <v>9461.2000000000007</v>
       </c>
       <c r="E3">
-        <v>11480.5</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+        <v>9340.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7255.1</v>
+        <v>5971.6</v>
       </c>
       <c r="C4">
-        <v>7185.2</v>
+        <v>5780.7</v>
       </c>
       <c r="D4">
-        <v>7205.5</v>
+        <v>5954.9</v>
       </c>
       <c r="E4">
-        <v>7222.2</v>
-      </c>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+        <v>5787.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5249.6</v>
+        <v>4337.6000000000004</v>
       </c>
       <c r="C5">
-        <v>5255.9</v>
+        <v>4871.8</v>
       </c>
       <c r="D5">
-        <v>5302.6</v>
+        <v>5201.5</v>
       </c>
       <c r="E5">
-        <v>5282.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+        <v>4150.6000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4154.2</v>
+        <v>3392.7</v>
       </c>
       <c r="C6">
-        <v>4046.8</v>
+        <v>4063.1</v>
       </c>
       <c r="D6">
-        <v>4682.5</v>
+        <v>4725.2</v>
       </c>
       <c r="E6">
-        <v>4318.3999999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+        <v>3195.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>4740.7</v>
+        <v>4375.1000000000004</v>
       </c>
       <c r="C7">
-        <v>4661.6000000000004</v>
+        <v>4602.6000000000004</v>
       </c>
       <c r="D7">
-        <v>4574</v>
+        <v>4710.3999999999996</v>
       </c>
       <c r="E7">
-        <v>4524</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+        <v>4322.6000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>4019.4</v>
+        <v>3721.8</v>
       </c>
       <c r="C8">
-        <v>3979.1</v>
+        <v>3943.7</v>
       </c>
       <c r="D8">
-        <v>4089.1</v>
+        <v>4183.2</v>
       </c>
       <c r="E8">
-        <v>4099.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+        <v>3878</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>3373.1</v>
+        <v>3179.8</v>
       </c>
       <c r="C9">
-        <v>3323.1</v>
+        <v>3335.1</v>
       </c>
       <c r="D9">
-        <v>3472.3</v>
+        <v>3539.5</v>
       </c>
       <c r="E9">
-        <v>3435.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+        <v>3214.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3141.9</v>
+        <v>2993.3</v>
       </c>
       <c r="C10">
-        <v>3092.1</v>
+        <v>3103.8</v>
       </c>
       <c r="D10">
-        <v>2980.2</v>
+        <v>3076.2</v>
       </c>
       <c r="E10">
-        <v>2961.7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+        <v>2749.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>3509.8</v>
+        <v>3061.8</v>
       </c>
       <c r="C11">
-        <v>3470.1</v>
+        <v>3418.8</v>
       </c>
       <c r="D11">
-        <v>3602.4</v>
+        <v>3709.7</v>
       </c>
       <c r="E11">
-        <v>3570.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+        <v>3322</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>3420.7</v>
+        <v>3109.6</v>
       </c>
       <c r="C12">
-        <v>3353.8</v>
+        <v>3226.5</v>
       </c>
       <c r="D12">
-        <v>3463.2</v>
+        <v>3563.6</v>
       </c>
       <c r="E12">
-        <v>3457.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+        <v>3116.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>3347</v>
+        <v>3197.7</v>
       </c>
       <c r="C13">
-        <v>3165.8</v>
+        <v>2999.1</v>
       </c>
       <c r="D13">
-        <v>3223</v>
+        <v>3347.9</v>
       </c>
       <c r="E13">
-        <v>3195.4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+        <v>2869.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>3104</v>
+        <v>3151.8</v>
       </c>
       <c r="C14">
-        <v>3275.5</v>
+        <v>2895.3</v>
       </c>
       <c r="D14">
-        <v>3068</v>
+        <v>3201.6</v>
       </c>
       <c r="E14">
-        <v>3053</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+        <v>2710.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>3316.1</v>
+        <v>3152.3</v>
       </c>
       <c r="C15">
-        <v>3244</v>
+        <v>3073.4</v>
       </c>
       <c r="D15">
-        <v>3398.6</v>
+        <v>3473.7</v>
       </c>
       <c r="E15">
-        <v>3405.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+        <v>3278.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>3116.3</v>
+        <v>3110.5</v>
       </c>
       <c r="C16">
-        <v>3179.4</v>
+        <v>2925.6</v>
       </c>
       <c r="D16">
-        <v>3220.3</v>
+        <v>3302.1</v>
       </c>
       <c r="E16">
-        <v>3189.5</v>
+        <v>3057.7</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
@@ -4225,16 +4754,16 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>2907.6</v>
+        <v>3029</v>
       </c>
       <c r="C17">
-        <v>3090.3</v>
+        <v>2760.1</v>
       </c>
       <c r="D17">
-        <v>2990.1</v>
+        <v>3114.8</v>
       </c>
       <c r="E17">
-        <v>2971.1</v>
+        <v>2809.4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
@@ -4242,16 +4771,16 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>2834.5</v>
+        <v>3008.1</v>
       </c>
       <c r="C18">
-        <v>2906.7</v>
+        <v>2689.1</v>
       </c>
       <c r="D18">
-        <v>2801</v>
+        <v>2953</v>
       </c>
       <c r="E18">
-        <v>2785.4</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
@@ -4259,16 +4788,16 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>2900.5</v>
+        <v>2994.4</v>
       </c>
       <c r="C19">
-        <v>3001.2</v>
+        <v>2814.1</v>
       </c>
       <c r="D19">
-        <v>3127.4</v>
+        <v>3216.1</v>
       </c>
       <c r="E19">
-        <v>3105.3</v>
+        <v>2932.9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
@@ -4276,16 +4805,16 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>2859.9</v>
+        <v>2988.1</v>
       </c>
       <c r="C20">
-        <v>2984.3</v>
+        <v>2751.8</v>
       </c>
       <c r="D20">
-        <v>3052.8</v>
+        <v>3203.6</v>
       </c>
       <c r="E20">
-        <v>3032.4</v>
+        <v>2829.8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
@@ -4293,16 +4822,16 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>2796.3</v>
+        <v>2990.2</v>
       </c>
       <c r="C21">
-        <v>2904.1</v>
+        <v>2690.3</v>
       </c>
       <c r="D21">
-        <v>2951.7</v>
+        <v>3198.6</v>
       </c>
       <c r="E21">
-        <v>2921.2</v>
+        <v>2710.3</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
@@ -4310,16 +4839,16 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>2782.9</v>
+        <v>2996.7</v>
       </c>
       <c r="C22">
-        <v>2885.1</v>
+        <v>2701.9</v>
       </c>
       <c r="D22">
-        <v>2869.3</v>
+        <v>3196.7</v>
       </c>
       <c r="E22">
-        <v>2862.9</v>
+        <v>2629.2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
@@ -4327,16 +4856,16 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>2729.9</v>
+        <v>2984.4</v>
       </c>
       <c r="C23">
-        <v>2954.5</v>
+        <v>2798.3</v>
       </c>
       <c r="D23">
-        <v>3100.3</v>
+        <v>3196.4</v>
       </c>
       <c r="E23">
-        <v>3057</v>
+        <v>2944.6</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.45">
@@ -4344,16 +4873,16 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>2676.4</v>
+        <v>2963.3</v>
       </c>
       <c r="C24">
-        <v>2891.6</v>
+        <v>2722.8</v>
       </c>
       <c r="D24">
-        <v>2979.3</v>
+        <v>3158.2</v>
       </c>
       <c r="E24">
-        <v>2949.3</v>
+        <v>2828.2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.45">
@@ -4361,16 +4890,16 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>2612.9</v>
+        <v>2941.6</v>
       </c>
       <c r="C25">
-        <v>2781.5</v>
+        <v>2643.6</v>
       </c>
       <c r="D25">
-        <v>2845.4</v>
+        <v>3090.3</v>
       </c>
       <c r="E25">
-        <v>2825.9</v>
+        <v>2682.3</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.45">
@@ -4378,16 +4907,16 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>2612.9</v>
+        <v>2918.8</v>
       </c>
       <c r="C26">
-        <v>2775.3</v>
+        <v>2624</v>
       </c>
       <c r="D26">
-        <v>2741.6</v>
+        <v>3035.5</v>
       </c>
       <c r="E26">
-        <v>2720.6</v>
+        <v>2572.9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.45">
@@ -4395,16 +4924,16 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>2603.5</v>
+        <v>2907.3</v>
       </c>
       <c r="C27">
-        <v>2845</v>
+        <v>2691.5</v>
       </c>
       <c r="D27">
-        <v>2953</v>
+        <v>3204.8</v>
       </c>
       <c r="E27">
-        <v>2930</v>
+        <v>2786.6</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.45">
@@ -4412,16 +4941,16 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2591.1999999999998</v>
+        <v>2899.2</v>
       </c>
       <c r="C28">
-        <v>2838.2</v>
+        <v>2659.8</v>
       </c>
       <c r="D28">
-        <v>2896</v>
+        <v>3204.5</v>
       </c>
       <c r="E28">
-        <v>2867.4</v>
+        <v>2710.3</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.45">
@@ -4429,16 +4958,16 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>2589.1999999999998</v>
+        <v>2898</v>
       </c>
       <c r="C29">
-        <v>2790.5</v>
+        <v>2619</v>
       </c>
       <c r="D29">
-        <v>2823.2</v>
+        <v>3215.8</v>
       </c>
       <c r="E29">
-        <v>2797.1</v>
+        <v>2619.3000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.45">
@@ -4446,16 +4975,16 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>2604.4</v>
+        <v>2898.4</v>
       </c>
       <c r="C30">
-        <v>2798</v>
+        <v>2642.3</v>
       </c>
       <c r="D30">
-        <v>2789.8</v>
+        <v>3225.2</v>
       </c>
       <c r="E30">
-        <v>2775.2</v>
+        <v>2574.9</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.45">
@@ -4463,16 +4992,16 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>2591.5</v>
+        <v>2899.3</v>
       </c>
       <c r="C31">
-        <v>2834.9</v>
+        <v>2689.1</v>
       </c>
       <c r="D31">
-        <v>2942.3</v>
+        <v>3196.7</v>
       </c>
       <c r="E31">
-        <v>2917.7</v>
+        <v>2773.2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.45">
@@ -4480,16 +5009,16 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>2593.6999999999998</v>
+        <v>2884.6</v>
       </c>
       <c r="C32">
-        <v>2793.2</v>
+        <v>2647.8</v>
       </c>
       <c r="D32">
-        <v>2865.1</v>
+        <v>3151.9</v>
       </c>
       <c r="E32">
-        <v>2846.3</v>
+        <v>2738.1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.45">
@@ -4497,16 +5026,16 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>2567.5</v>
+        <v>2880.6</v>
       </c>
       <c r="C33">
-        <v>2729.1</v>
+        <v>2600.1</v>
       </c>
       <c r="D33">
-        <v>2807.9</v>
+        <v>3096.4</v>
       </c>
       <c r="E33">
-        <v>2758.9</v>
+        <v>2631.7</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.45">
@@ -4514,16 +5043,16 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>2567.1</v>
+        <v>2868.2</v>
       </c>
       <c r="C34">
-        <v>2733.3</v>
+        <v>2594.4</v>
       </c>
       <c r="D34">
-        <v>2707.6</v>
+        <v>3066.4</v>
       </c>
       <c r="E34">
-        <v>2686.3</v>
+        <v>2547.9</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.45">
@@ -4531,16 +5060,16 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>2682.9</v>
+        <v>2867.6</v>
       </c>
       <c r="C35">
-        <v>2770.6</v>
+        <v>2637.4</v>
       </c>
       <c r="D35">
-        <v>2873.9</v>
+        <v>3167.5</v>
       </c>
       <c r="E35">
-        <v>2845.1</v>
+        <v>2718.5</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.45">
@@ -4548,16 +5077,16 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>2588.6</v>
+        <v>2861.1</v>
       </c>
       <c r="C36">
-        <v>2774.7</v>
+        <v>2614.1</v>
       </c>
       <c r="D36">
-        <v>2815.4</v>
+        <v>3168.7</v>
       </c>
       <c r="E36">
-        <v>2786.3</v>
+        <v>2650.4</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.45">
@@ -4565,16 +5094,16 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>2590.6999999999998</v>
+        <v>2854.4</v>
       </c>
       <c r="C37">
-        <v>2766</v>
+        <v>2587.9</v>
       </c>
       <c r="D37">
-        <v>2773.2</v>
+        <v>3162.8</v>
       </c>
       <c r="E37">
-        <v>2744.6</v>
+        <v>2585</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.45">
@@ -4582,16 +5111,16 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>2577.6</v>
+        <v>2860.7</v>
       </c>
       <c r="C38">
-        <v>2785.6</v>
+        <v>2641.8</v>
       </c>
       <c r="D38">
-        <v>2752.2</v>
+        <v>3160.6</v>
       </c>
       <c r="E38">
-        <v>2730.5</v>
+        <v>2553.1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.45">
@@ -4599,16 +5128,16 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>2554</v>
+        <v>2854.7</v>
       </c>
       <c r="C39">
-        <v>2775.3</v>
+        <v>2651.2</v>
       </c>
       <c r="D39">
-        <v>2852</v>
+        <v>3140.7</v>
       </c>
       <c r="E39">
-        <v>2836.4</v>
+        <v>2726</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.45">
@@ -4616,16 +5145,16 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>2531.9</v>
+        <v>2851.9</v>
       </c>
       <c r="C40">
-        <v>2750.8</v>
+        <v>2613.3000000000002</v>
       </c>
       <c r="D40">
-        <v>2810.2</v>
+        <v>3110.5</v>
       </c>
       <c r="E40">
-        <v>2794.1</v>
+        <v>2665.4</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.45">
@@ -4633,16 +5162,16 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>2511.6999999999998</v>
+        <v>2877.5</v>
       </c>
       <c r="C41">
-        <v>2707.1</v>
+        <v>2578.9</v>
       </c>
       <c r="D41">
-        <v>2743.1</v>
+        <v>3066.8</v>
       </c>
       <c r="E41">
-        <v>2724.3</v>
+        <v>2589.9</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.45">
@@ -4650,16 +5179,16 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>2506.9</v>
+        <v>2842.9</v>
       </c>
       <c r="C42">
-        <v>2737</v>
+        <v>2580.6999999999998</v>
       </c>
       <c r="D42">
-        <v>2693.8</v>
+        <v>3054.5</v>
       </c>
       <c r="E42">
-        <v>2672.4</v>
+        <v>2535.1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.45">
@@ -4667,16 +5196,16 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>2495.9</v>
+        <v>2838.9</v>
       </c>
       <c r="C43">
-        <v>2742.4</v>
+        <v>2611.6</v>
       </c>
       <c r="D43">
-        <v>2812.5</v>
+        <v>3106.1</v>
       </c>
       <c r="E43">
-        <v>2789.7</v>
+        <v>2684.8</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.45">
@@ -4684,16 +5213,16 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>2493.6</v>
+        <v>2831.4</v>
       </c>
       <c r="C44">
-        <v>2732.6</v>
+        <v>2600.6999999999998</v>
       </c>
       <c r="D44">
-        <v>2784.1</v>
+        <v>3123.1</v>
       </c>
       <c r="E44">
-        <v>2773.9</v>
+        <v>2664.5</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.45">
@@ -4701,16 +5230,16 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>2492.9</v>
+        <v>2830.1</v>
       </c>
       <c r="C45">
-        <v>2715.3</v>
+        <v>2587.4</v>
       </c>
       <c r="D45">
-        <v>2741.2</v>
+        <v>3120.1</v>
       </c>
       <c r="E45">
-        <v>2725.7</v>
+        <v>2570.1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.45">
@@ -4718,16 +5247,16 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>2478.9</v>
+        <v>2831.7</v>
       </c>
       <c r="C46">
-        <v>2734.5</v>
+        <v>2634.3</v>
       </c>
       <c r="D46">
-        <v>2733.6</v>
+        <v>3104.6</v>
       </c>
       <c r="E46">
-        <v>2705.6</v>
+        <v>2547.6999999999998</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.45">
@@ -4735,16 +5264,16 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>2465.1</v>
+        <v>2831.9</v>
       </c>
       <c r="C47">
-        <v>2745.4</v>
+        <v>2623.8</v>
       </c>
       <c r="D47">
-        <v>2797</v>
+        <v>3084.8</v>
       </c>
       <c r="E47">
-        <v>2783.7</v>
+        <v>2667.8</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.45">
@@ -4752,16 +5281,16 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>2456.1999999999998</v>
+        <v>2830</v>
       </c>
       <c r="C48">
-        <v>2724</v>
+        <v>2607.1</v>
       </c>
       <c r="D48">
-        <v>2770.3</v>
+        <v>3057.7</v>
       </c>
       <c r="E48">
-        <v>2752.5</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.45">
@@ -4769,16 +5298,16 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>2436</v>
+        <v>2841.2</v>
       </c>
       <c r="C49">
-        <v>2689</v>
+        <v>2583.3000000000002</v>
       </c>
       <c r="D49">
-        <v>2720.3</v>
+        <v>3025.8</v>
       </c>
       <c r="E49">
-        <v>2694.4</v>
+        <v>2586.6999999999998</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
@@ -4786,16 +5315,16 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>2440</v>
+        <v>2830.3</v>
       </c>
       <c r="C50">
-        <v>2702.8</v>
+        <v>2584.4</v>
       </c>
       <c r="D50">
-        <v>2685.7</v>
+        <v>3011.4</v>
       </c>
       <c r="E50">
-        <v>2658.6</v>
+        <v>2532.4</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
@@ -4803,16 +5332,16 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>2437.8000000000002</v>
+        <v>2831.6</v>
       </c>
       <c r="C51">
-        <v>2718</v>
+        <v>2612.5</v>
       </c>
       <c r="D51">
-        <v>2785</v>
+        <v>3072.1</v>
       </c>
       <c r="E51">
-        <v>2767.5</v>
+        <v>2643.9</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
@@ -4820,16 +5349,16 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>2426.4</v>
+        <v>2824.3</v>
       </c>
       <c r="C52">
-        <v>2704.1</v>
+        <v>2585.4</v>
       </c>
       <c r="D52">
-        <v>2737.5</v>
+        <v>3066.1</v>
       </c>
       <c r="E52">
-        <v>2759.4</v>
+        <v>2593.3000000000002</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.45">
@@ -4837,16 +5366,16 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>2427.6</v>
+        <v>2824.4</v>
       </c>
       <c r="C53">
-        <v>2687.5</v>
+        <v>2581</v>
       </c>
       <c r="D53">
-        <v>2714.4</v>
+        <v>3054.8</v>
       </c>
       <c r="E53">
-        <v>2690.9</v>
+        <v>2554.4</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.45">
@@ -4854,16 +5383,16 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>2442.4</v>
+        <v>2824.5</v>
       </c>
       <c r="C54">
-        <v>2702</v>
+        <v>2599.1</v>
       </c>
       <c r="D54">
-        <v>2727.6</v>
+        <v>3054.1</v>
       </c>
       <c r="E54">
-        <v>2676.3</v>
+        <v>2534.9</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.45">
@@ -4871,16 +5400,16 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>2421.5</v>
+        <v>2822.5</v>
       </c>
       <c r="C55">
-        <v>2717.8</v>
+        <v>2610.6</v>
       </c>
       <c r="D55">
-        <v>2748.4</v>
+        <v>3039</v>
       </c>
       <c r="E55">
-        <v>2740</v>
+        <v>2629.1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.45">
@@ -4888,16 +5417,16 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>2410.8000000000002</v>
+        <v>2822.3</v>
       </c>
       <c r="C56">
-        <v>2686.9</v>
+        <v>2598.3000000000002</v>
       </c>
       <c r="D56">
-        <v>2728.9</v>
+        <v>3010.3</v>
       </c>
       <c r="E56">
-        <v>2713</v>
+        <v>2609.1</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.45">
@@ -4905,16 +5434,16 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>2416.1</v>
+        <v>2823.5</v>
       </c>
       <c r="C57">
-        <v>2676.3</v>
+        <v>2577.6</v>
       </c>
       <c r="D57">
-        <v>2702.5</v>
+        <v>3002</v>
       </c>
       <c r="E57">
-        <v>2673.6</v>
+        <v>2555.5</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.45">
@@ -4922,16 +5451,16 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>2430.1</v>
+        <v>2825</v>
       </c>
       <c r="C58">
-        <v>2703.4</v>
+        <v>2592.3000000000002</v>
       </c>
       <c r="D58">
-        <v>2691</v>
+        <v>3012.5</v>
       </c>
       <c r="E58">
-        <v>2662.7</v>
+        <v>2530.1999999999998</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.45">
@@ -4939,16 +5468,16 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>2419.6999999999998</v>
+        <v>2824</v>
       </c>
       <c r="C59">
-        <v>2707</v>
+        <v>3423.9</v>
       </c>
       <c r="D59">
-        <v>2755.4</v>
+        <v>3040.5</v>
       </c>
       <c r="E59">
-        <v>2743.6</v>
+        <v>2614.5</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.45">
@@ -4956,16 +5485,16 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>2419</v>
+        <v>2826.4</v>
       </c>
       <c r="C60">
-        <v>2692.2</v>
+        <v>2708.3</v>
       </c>
       <c r="D60">
-        <v>2713.1</v>
+        <v>3030.8</v>
       </c>
       <c r="E60">
-        <v>2694.3</v>
+        <v>2572.9</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.45">
@@ -4973,16 +5502,16 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>2407.3000000000002</v>
+        <v>2827.8</v>
       </c>
       <c r="C61">
-        <v>2695.1</v>
+        <v>2686</v>
       </c>
       <c r="D61">
-        <v>2709.5</v>
+        <v>3064.1</v>
       </c>
       <c r="E61">
-        <v>2688.7</v>
+        <v>2556.8000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.45">
@@ -4990,16 +5519,16 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>2406.4</v>
+        <v>2823.8</v>
       </c>
       <c r="C62">
-        <v>2696</v>
+        <v>2626.9</v>
       </c>
       <c r="D62">
-        <v>2732.5</v>
+        <v>3043.6</v>
       </c>
       <c r="E62">
-        <v>2706.9</v>
+        <v>2536.1999999999998</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.45">
@@ -5007,16 +5536,16 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>2373.5</v>
+        <v>2850.7</v>
       </c>
       <c r="C63">
-        <v>2701</v>
+        <v>2610.8000000000002</v>
       </c>
       <c r="D63">
-        <v>2722.3</v>
+        <v>3010.1</v>
       </c>
       <c r="E63">
-        <v>2718</v>
+        <v>2611.3000000000002</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.45">
@@ -5024,16 +5553,16 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>2374.6999999999998</v>
+        <v>2827.2</v>
       </c>
       <c r="C64">
-        <v>2677.5</v>
+        <v>2603.5</v>
       </c>
       <c r="D64">
-        <v>2712.1</v>
+        <v>2996.1</v>
       </c>
       <c r="E64">
-        <v>2716.2</v>
+        <v>2586.1999999999998</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.45">
@@ -5041,16 +5570,16 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>2361</v>
+        <v>2827.2</v>
       </c>
       <c r="C65">
-        <v>2665.3</v>
+        <v>2585.6999999999998</v>
       </c>
       <c r="D65">
-        <v>2690.8</v>
+        <v>2991.3</v>
       </c>
       <c r="E65">
-        <v>2674.7</v>
+        <v>2548.6</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.45">
@@ -5058,16 +5587,16 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>2355.3000000000002</v>
+        <v>2824.2</v>
       </c>
       <c r="C66">
-        <v>2689.7</v>
+        <v>2597.5</v>
       </c>
       <c r="D66">
-        <v>2674.6</v>
+        <v>2968.6</v>
       </c>
       <c r="E66">
-        <v>2649.9</v>
+        <v>2526.4</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.45">
@@ -5075,16 +5604,16 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>2351.9</v>
+        <v>2824.5</v>
       </c>
       <c r="C67">
-        <v>2686.4</v>
+        <v>2607.6999999999998</v>
       </c>
       <c r="D67">
-        <v>2722.4</v>
+        <v>2999.5</v>
       </c>
       <c r="E67">
-        <v>2701.9</v>
+        <v>2598.4</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.45">
@@ -5092,16 +5621,16 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>2343.8000000000002</v>
+        <v>2828</v>
       </c>
       <c r="C68">
-        <v>2680.1</v>
+        <v>2603.6999999999998</v>
       </c>
       <c r="D68">
-        <v>2707.3</v>
+        <v>3004.8</v>
       </c>
       <c r="E68">
-        <v>2698.9</v>
+        <v>2572.1</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.45">
@@ -5109,16 +5638,16 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>2342.6</v>
+        <v>2828.4</v>
       </c>
       <c r="C69">
-        <v>2672.4</v>
+        <v>2604.1</v>
       </c>
       <c r="D69">
-        <v>2688.9</v>
+        <v>3007.1</v>
       </c>
       <c r="E69">
-        <v>2669.7</v>
+        <v>2544.6</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.45">
@@ -5126,16 +5655,16 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>2345.5</v>
+        <v>2828.5</v>
       </c>
       <c r="C70">
-        <v>2691.7</v>
+        <v>2615.1</v>
       </c>
       <c r="D70">
-        <v>2722.5</v>
+        <v>2988.1</v>
       </c>
       <c r="E70">
-        <v>2679</v>
+        <v>2531.1</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.45">
@@ -5143,16 +5672,16 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>2337.1</v>
+        <v>2826.6</v>
       </c>
       <c r="C71">
-        <v>2685.6</v>
+        <v>2612.5</v>
       </c>
       <c r="D71">
-        <v>2693.5</v>
+        <v>2983.5</v>
       </c>
       <c r="E71">
-        <v>2689</v>
+        <v>2583.6999999999998</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.45">
@@ -5160,16 +5689,16 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>2335</v>
+        <v>2829.8</v>
       </c>
       <c r="C72">
-        <v>2676.5</v>
+        <v>2606.6</v>
       </c>
       <c r="D72">
-        <v>2701</v>
+        <v>2973.8</v>
       </c>
       <c r="E72">
-        <v>2680.7</v>
+        <v>2560.5</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.45">
@@ -5177,16 +5706,16 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>2325.1</v>
+        <v>2829.4</v>
       </c>
       <c r="C73">
-        <v>2671.7</v>
+        <v>2594.1</v>
       </c>
       <c r="D73">
-        <v>2678.6</v>
+        <v>2957.7</v>
       </c>
       <c r="E73">
-        <v>2657.8</v>
+        <v>2539.6999999999998</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.45">
@@ -5194,16 +5723,16 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>2333.9</v>
+        <v>2831.5</v>
       </c>
       <c r="C74">
-        <v>2702.6</v>
+        <v>2608.3000000000002</v>
       </c>
       <c r="D74">
-        <v>2671.5</v>
+        <v>2959.6</v>
       </c>
       <c r="E74">
-        <v>2653.8</v>
+        <v>2532.5</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.45">
@@ -5211,16 +5740,16 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>2326.9</v>
+        <v>3010.2</v>
       </c>
       <c r="C75">
-        <v>2686.2</v>
+        <v>2614.3000000000002</v>
       </c>
       <c r="D75">
-        <v>2699.5</v>
+        <v>2978</v>
       </c>
       <c r="E75">
-        <v>2681.3</v>
+        <v>2566.1999999999998</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.45">
@@ -5228,16 +5757,16 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>2322.1999999999998</v>
+        <v>3070.8</v>
       </c>
       <c r="C76">
-        <v>2674.9</v>
+        <v>2606.3000000000002</v>
       </c>
       <c r="D76">
-        <v>2684.7</v>
+        <v>2978.9</v>
       </c>
       <c r="E76">
-        <v>2664</v>
+        <v>2547.3000000000002</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.45">
@@ -5245,16 +5774,16 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>2310.4</v>
+        <v>3073.8</v>
       </c>
       <c r="C77">
-        <v>2669.7</v>
+        <v>2602.8000000000002</v>
       </c>
       <c r="D77">
-        <v>2671.7</v>
+        <v>2982.2</v>
       </c>
       <c r="E77">
-        <v>2710.5</v>
+        <v>2537.9</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.45">
@@ -5262,16 +5791,16 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>2319.8000000000002</v>
+        <v>3088.3</v>
       </c>
       <c r="C78">
-        <v>2682.5</v>
+        <v>2618.4</v>
       </c>
       <c r="D78">
-        <v>2706.1</v>
+        <v>2978.4</v>
       </c>
       <c r="E78">
-        <v>2675.8</v>
+        <v>2534.6</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.45">
@@ -5279,16 +5808,16 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>2312.6</v>
+        <v>2867.3</v>
       </c>
       <c r="C79">
-        <v>2679.1</v>
+        <v>2619.4</v>
       </c>
       <c r="D79">
-        <v>2694.5</v>
+        <v>2973.7</v>
       </c>
       <c r="E79">
-        <v>2678.3</v>
+        <v>2566.3000000000002</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.45">
@@ -5296,16 +5825,16 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>2305.1999999999998</v>
+        <v>2833.1</v>
       </c>
       <c r="C80">
-        <v>2669.8</v>
+        <v>2604.6999999999998</v>
       </c>
       <c r="D80">
-        <v>2685.8</v>
+        <v>2962.6</v>
       </c>
       <c r="E80">
-        <v>2663.1</v>
+        <v>2563.8000000000002</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.45">
@@ -5313,16 +5842,16 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>2299.6</v>
+        <v>2833.1</v>
       </c>
       <c r="C81">
-        <v>2668.2</v>
+        <v>2599.1999999999998</v>
       </c>
       <c r="D81">
-        <v>2677.3</v>
+        <v>2961</v>
       </c>
       <c r="E81">
-        <v>2658.2</v>
+        <v>2539.5</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.45">
@@ -5330,16 +5859,16 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>2292.4</v>
+        <v>2836</v>
       </c>
       <c r="C82">
-        <v>2679.4</v>
+        <v>2646.7</v>
       </c>
       <c r="D82">
-        <v>2658.8</v>
+        <v>2944</v>
       </c>
       <c r="E82">
-        <v>2639.6</v>
+        <v>2517.4</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.45">
@@ -5347,16 +5876,16 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>2290.4</v>
+        <v>2837.9</v>
       </c>
       <c r="C83">
-        <v>2672</v>
+        <v>2650.8</v>
       </c>
       <c r="D83">
-        <v>2706.3</v>
+        <v>2978.1</v>
       </c>
       <c r="E83">
-        <v>2685.3</v>
+        <v>2572.6</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.45">
@@ -5364,16 +5893,16 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>2300.9</v>
+        <v>2841.1</v>
       </c>
       <c r="C84">
-        <v>2680.4</v>
+        <v>2644.5</v>
       </c>
       <c r="D84">
-        <v>2698.1</v>
+        <v>2978.6</v>
       </c>
       <c r="E84">
-        <v>2669.1</v>
+        <v>2549.6</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.45">
@@ -5381,16 +5910,16 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>2302.5</v>
+        <v>2838.7</v>
       </c>
       <c r="C85">
-        <v>2671.9</v>
+        <v>2606.1999999999998</v>
       </c>
       <c r="D85">
-        <v>2739.4</v>
+        <v>2985.2</v>
       </c>
       <c r="E85">
-        <v>2675.2</v>
+        <v>2534.1999999999998</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.45">
@@ -5398,16 +5927,16 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>2287.6999999999998</v>
+        <v>2839</v>
       </c>
       <c r="C86">
-        <v>2654.3</v>
+        <v>2599.8000000000002</v>
       </c>
       <c r="D86">
-        <v>2707.1</v>
+        <v>2987.8</v>
       </c>
       <c r="E86">
-        <v>2689</v>
+        <v>2549.5</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.45">
@@ -5415,16 +5944,16 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>2282.9</v>
+        <v>2841.5</v>
       </c>
       <c r="C87">
-        <v>2670.8</v>
+        <v>2616.8000000000002</v>
       </c>
       <c r="D87">
-        <v>2697.9</v>
+        <v>2971.1</v>
       </c>
       <c r="E87">
-        <v>2673.4</v>
+        <v>2564.3000000000002</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.45">
@@ -5432,16 +5961,16 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>2281.9</v>
+        <v>2838.2</v>
       </c>
       <c r="C88">
-        <v>2673.6</v>
+        <v>2616.4</v>
       </c>
       <c r="D88">
-        <v>2700.7</v>
+        <v>2972.2</v>
       </c>
       <c r="E88">
-        <v>2678</v>
+        <v>2552.8000000000002</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.45">
@@ -5449,16 +5978,16 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>2278.4</v>
+        <v>2836.7</v>
       </c>
       <c r="C89">
-        <v>2662.9</v>
+        <v>2609.1</v>
       </c>
       <c r="D89">
-        <v>2670.1</v>
+        <v>2958.7</v>
       </c>
       <c r="E89">
-        <v>2650.1</v>
+        <v>2545.4</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.45">
@@ -5466,16 +5995,16 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>2280.6999999999998</v>
+        <v>2838.6</v>
       </c>
       <c r="C90">
-        <v>2660.7</v>
+        <v>2602.6</v>
       </c>
       <c r="D90">
-        <v>2660</v>
+        <v>2953.5</v>
       </c>
       <c r="E90">
-        <v>2652</v>
+        <v>2535.4</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.45">
@@ -5483,16 +6012,16 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>2283.1</v>
+        <v>2843.2</v>
       </c>
       <c r="C91">
-        <v>2681.8</v>
+        <v>2613.9</v>
       </c>
       <c r="D91">
-        <v>2696.3</v>
+        <v>2969.3</v>
       </c>
       <c r="E91">
-        <v>2670.4</v>
+        <v>2560.8000000000002</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.45">
@@ -5500,16 +6029,16 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>2291.8000000000002</v>
+        <v>2841.6</v>
       </c>
       <c r="C92">
-        <v>2675.5</v>
+        <v>2616.1</v>
       </c>
       <c r="D92">
-        <v>2690.4</v>
+        <v>2961.9</v>
       </c>
       <c r="E92">
-        <v>2647.4</v>
+        <v>2531.8000000000002</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.45">
@@ -5517,16 +6046,16 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>2311.3000000000002</v>
+        <v>2839.4</v>
       </c>
       <c r="C93">
-        <v>2665.3</v>
+        <v>2612.5</v>
       </c>
       <c r="D93">
-        <v>2660.5</v>
+        <v>2966.7</v>
       </c>
       <c r="E93">
-        <v>2642</v>
+        <v>2523.6</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.45">
@@ -5534,16 +6063,16 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>2285.1999999999998</v>
+        <v>2894.6</v>
       </c>
       <c r="C94">
-        <v>2662.7</v>
+        <v>2609.5</v>
       </c>
       <c r="D94">
-        <v>2695.9</v>
+        <v>2960.3</v>
       </c>
       <c r="E94">
-        <v>2669.1</v>
+        <v>2549.8000000000002</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.45">
@@ -5551,16 +6080,16 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>2290.9</v>
+        <v>2857.4</v>
       </c>
       <c r="C95">
-        <v>2658.8</v>
+        <v>2614.6999999999998</v>
       </c>
       <c r="D95">
-        <v>2675.9</v>
+        <v>2957.2</v>
       </c>
       <c r="E95">
-        <v>2665.3</v>
+        <v>2545</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.45">
@@ -5568,16 +6097,16 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>2293.4</v>
+        <v>2880</v>
       </c>
       <c r="C96">
-        <v>2695.4</v>
+        <v>2623.6</v>
       </c>
       <c r="D96">
-        <v>2690.1</v>
+        <v>2968.8</v>
       </c>
       <c r="E96">
-        <v>2675.2</v>
+        <v>2549.5</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.45">
@@ -5585,16 +6114,16 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>2301.1999999999998</v>
+        <v>2842.9</v>
       </c>
       <c r="C97">
-        <v>2668.1</v>
+        <v>2615.9</v>
       </c>
       <c r="D97">
-        <v>2670.3</v>
+        <v>2958</v>
       </c>
       <c r="E97">
-        <v>2647</v>
+        <v>2535.1999999999998</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.45">
@@ -5602,16 +6131,16 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>2281.1</v>
+        <v>2842.1</v>
       </c>
       <c r="C98">
-        <v>2669</v>
+        <v>2611.8000000000002</v>
       </c>
       <c r="D98">
-        <v>2660.4</v>
+        <v>2954.5</v>
       </c>
       <c r="E98">
-        <v>2642.6</v>
+        <v>2524.6</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.45">
@@ -5619,16 +6148,16 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>2278.4</v>
+        <v>2845.8</v>
       </c>
       <c r="C99">
-        <v>2669.7</v>
+        <v>2612.9</v>
       </c>
       <c r="D99">
-        <v>2693.2</v>
+        <v>2972.7</v>
       </c>
       <c r="E99">
-        <v>2674.8</v>
+        <v>2600.3000000000002</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.45">
@@ -5636,16 +6165,16 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>2269.5</v>
+        <v>2844</v>
       </c>
       <c r="C100">
-        <v>2667.3</v>
+        <v>2623.1</v>
       </c>
       <c r="D100">
-        <v>2672</v>
+        <v>2964.8</v>
       </c>
       <c r="E100">
-        <v>2644.8</v>
+        <v>2535.3000000000002</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.45">
@@ -5653,16 +6182,16 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>2264.3000000000002</v>
+        <v>2844.1</v>
       </c>
       <c r="C101">
-        <v>2685.6</v>
+        <v>2619.9</v>
       </c>
       <c r="D101">
-        <v>2669.7</v>
+        <v>2956.6</v>
       </c>
       <c r="E101">
-        <v>2655.2</v>
+        <v>2527.8000000000002</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.45">
@@ -5670,16 +6199,16 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>2262.1</v>
+        <v>2844.7</v>
       </c>
       <c r="C102">
-        <v>2661.1</v>
+        <v>2612</v>
       </c>
       <c r="D102">
-        <v>2675.7</v>
+        <v>2960.2</v>
       </c>
       <c r="E102">
-        <v>2664.4</v>
+        <v>2527.3000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>